<commit_message>
Pavani Gandepalli status on 19/1/2021
</commit_message>
<xml_diff>
--- a/PavaniGandepalli/Pavani_Gandepalli_B&I_StatusSheet.xlsx
+++ b/PavaniGandepalli/Pavani_Gandepalli_B&I_StatusSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -93,6 +93,27 @@
   </si>
   <si>
     <t>On leave from 04-Jan-2021 to 07-Jan-2021</t>
+  </si>
+  <si>
+    <t>19/1/2021</t>
+  </si>
+  <si>
+    <t>C Hacker rank files</t>
+  </si>
+  <si>
+    <t>ArraySum.c
+VeryBigSum.c</t>
+  </si>
+  <si>
+    <t>Pyton Hacker Rank files</t>
+  </si>
+  <si>
+    <t>1.Practiced and added git commands in git cheat sheet
+2.Did 2 basic hacker rank programs in C
+3.Worked on memory layout in C as I couldn't answer questions in mock interview
+4. Learnt about why software testing is needed and some differences between manual testing and autoamtion testing before today's  Srinivasa session 
+5. Attended meeting "Softwate testing session by Srinivasa"
+6. Installing pycharm IDE in my PC</t>
   </si>
 </sst>
 </file>
@@ -185,7 +206,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -207,6 +227,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -513,149 +536,164 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="8" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" style="7" customWidth="1"/>
     <col min="2" max="2" width="41.85546875" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:5" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:5" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C7" s="9" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="11">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
         <v>44409</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
         <v>44501</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
         <v>44531</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+    <row r="14" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
+    <row r="15" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F21" s="5"/>
+      <c r="F21" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Pavani Gandepalli status on 20-Jan-2021
</commit_message>
<xml_diff>
--- a/PavaniGandepalli/Pavani_Gandepalli_B&I_StatusSheet.xlsx
+++ b/PavaniGandepalli/Pavani_Gandepalli_B&I_StatusSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -114,6 +114,23 @@
 4. Learnt about why software testing is needed and some differences between manual testing and autoamtion testing before today's  Srinivasa session 
 5. Attended meeting "Softwate testing session by Srinivasa"
 6. Installing pycharm IDE in my PC</t>
+  </si>
+  <si>
+    <t>20/1/2021</t>
+  </si>
+  <si>
+    <t>Flipping_Bits.txt
+Bitwise_Operators.txt</t>
+  </si>
+  <si>
+    <t>1. Added few more GIT commands in the cheat sheet
+2. Attended syncup meeting with Srivalli
+3. Completed bitwise operators in C and did 2 hacker rank programs on bitwise operators
+4. Completed defining and accessing members of structures
+5. Understand how memory is allocated for structures
+6. Completed how to define and access members of unions and understood memory allocation of members
+7. Understood bitfields 
+8. Attended meeting "Softwate testing session by Srinivasa"</t>
   </si>
 </sst>
 </file>
@@ -536,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,7 +562,7 @@
     <col min="1" max="1" width="19.85546875" style="7" customWidth="1"/>
     <col min="2" max="2" width="41.85546875" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -667,10 +684,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
+    <row r="16" spans="1:5" ht="225" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+      <c r="D16" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>

</xml_diff>

<commit_message>
Pavani Gandepalli Status on 21/Jan/2021
</commit_message>
<xml_diff>
--- a/PavaniGandepalli/Pavani_Gandepalli_B&I_StatusSheet.xlsx
+++ b/PavaniGandepalli/Pavani_Gandepalli_B&I_StatusSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Date</t>
   </si>
@@ -131,6 +131,23 @@
 6. Completed how to define and access members of unions and understood memory allocation of members
 7. Understood bitfields 
 8. Attended meeting "Softwate testing session by Srinivasa"</t>
+  </si>
+  <si>
+    <t>21/1/2021</t>
+  </si>
+  <si>
+    <t>BirthdayCake.txt</t>
+  </si>
+  <si>
+    <t>1. Learnt what is pointer, how to declare, initialize and access pointer variables
+2. What is NULL pointer
+3. Pointer Arthematic 
+4. Strings, How to declare, initialize and access strings
+5. Using %s, scanf, gets, puts, fgets for string input and optput
+6. Uderstood predefined functions in strings
+7. 2-D strings , memory allocation of strings 
+8. Completed one hacker rank program
+9. Attended session by Srinivasa</t>
   </si>
 </sst>
 </file>
@@ -553,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,27 +713,34 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
+    <row r="17" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D17" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F21" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pavani Gandepalli status on 28/1/2021
</commit_message>
<xml_diff>
--- a/PavaniGandepalli/Pavani_Gandepalli_B&I_StatusSheet.xlsx
+++ b/PavaniGandepalli/Pavani_Gandepalli_B&I_StatusSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Date</t>
   </si>
@@ -148,6 +148,40 @@
 7. 2-D strings , memory allocation of strings 
 8. Completed one hacker rank program
 9. Attended session by Srinivasa</t>
+  </si>
+  <si>
+    <t>22/1/2021</t>
+  </si>
+  <si>
+    <t>1. I have learnt syntax, if,if-else,elif ladder, for loop, basics in list and tuple as my interview profile needed python 
+2. Revision done on GIT and ADB commands 
+3. Attended the interview at 5PM and shared the interview question to the team</t>
+  </si>
+  <si>
+    <t>On leave 25/1/2021</t>
+  </si>
+  <si>
+    <t>27/1/2021</t>
+  </si>
+  <si>
+    <t>staircase.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Practiced different storage classes, and checked the size using size&lt;executable_file&gt; to check where the variable is storing 
+2. Worked on hacker rank program it took more time to get logic 
+3. Understand Bitwise operators and Completed 3 programs in Bitwise operators from givem list of programs </t>
+  </si>
+  <si>
+    <t>28/1/2021</t>
+  </si>
+  <si>
+    <t>1. Completed 5 programs in bitwise operators from given list
+2. Attended testing session at 10AM and Srinivas gave few tasks on testcases 
+3. Completed the task given by Srinivas and attended one more session at 2PM
+4. Completed on Hacker rank program in C</t>
+  </si>
+  <si>
+    <t>MinMax.txt</t>
   </si>
 </sst>
 </file>
@@ -234,7 +268,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -264,6 +298,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -570,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,22 +762,46 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="3"/>
+    <row r="18" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>33</v>
+      </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="3"/>
+    <row r="20" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D20" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="F21" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pavani Gandepalli status on 29/01/2021
</commit_message>
<xml_diff>
--- a/PavaniGandepalli/Pavani_Gandepalli_B&I_StatusSheet.xlsx
+++ b/PavaniGandepalli/Pavani_Gandepalli_B&I_StatusSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Date</t>
   </si>
@@ -182,6 +182,18 @@
   </si>
   <si>
     <t>MinMax.txt</t>
+  </si>
+  <si>
+    <t>29/1/2021</t>
+  </si>
+  <si>
+    <t>1. Attended time management session
+2. Completed 2 bitwise operators programs, 1 string program and  2 recursion programs from the given list
+3. Worked on task given by Srinivas regarding testing on my mobile 
+4. Completed one hacker rank program in C</t>
+  </si>
+  <si>
+    <t>MaximizingXor.txt</t>
   </si>
 </sst>
 </file>
@@ -605,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,6 +816,17 @@
       </c>
       <c r="F21" s="4"/>
     </row>
+    <row r="22" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Pavani Gandepalli daily status on Feb 1 2021
</commit_message>
<xml_diff>
--- a/PavaniGandepalli/Pavani_Gandepalli_B&I_StatusSheet.xlsx
+++ b/PavaniGandepalli/Pavani_Gandepalli_B&I_StatusSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Date</t>
   </si>
@@ -194,6 +194,17 @@
   </si>
   <si>
     <t>MaximizingXor.txt</t>
+  </si>
+  <si>
+    <t>FindDigits.txt
+FunctionsInC.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. I have completed bitwise operators 1 program, pointers 5 programs from given list of programs and pushed to github
+2. I worked on performance testing with linpack app, Vellamo app 
+3. I have worked on camera few Camera test cases and tested them on my mobile and recored the results
+4. Attended Srinivas session about test cases writing and validation of my 
+5. I have completed 2 hacker rank programs today </t>
   </si>
 </sst>
 </file>
@@ -617,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,6 +838,17 @@
         <v>42</v>
       </c>
     </row>
+    <row r="23" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
+        <v>44229</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Pavani Gandepalli daily status on 2/2/2021
</commit_message>
<xml_diff>
--- a/PavaniGandepalli/Pavani_Gandepalli_B&I_StatusSheet.xlsx
+++ b/PavaniGandepalli/Pavani_Gandepalli_B&I_StatusSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Date</t>
   </si>
@@ -205,6 +205,17 @@
 3. I have worked on camera few Camera test cases and tested them on my mobile and recored the results
 4. Attended Srinivas session about test cases writing and validation of my 
 5. I have completed 2 hacker rank programs today </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. I have completed 4 string programs and 6 recursion programs from the given list of C questions and pushed the programs into git https://github.com/gandepallipavani/C_Programs
+2. I worked on testcases writing for whatsapp as per the task given by Srinivas
+3. I worked on writing sample bug ticket in notepad as per the task given by Srinivas
+4. Attended the session by Srinivas about validating the testcases written
+5. Completed 2 hacker rank programs </t>
+  </si>
+  <si>
+    <t>PointersInC.txt
+ComditionalStatementsInC.txt</t>
   </si>
 </sst>
 </file>
@@ -628,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,6 +860,17 @@
         <v>43</v>
       </c>
     </row>
+    <row r="24" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>44229</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Pavani Gandepalli status on 3/2/2021
</commit_message>
<xml_diff>
--- a/PavaniGandepalli/Pavani_Gandepalli_B&I_StatusSheet.xlsx
+++ b/PavaniGandepalli/Pavani_Gandepalli_B&I_StatusSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Date</t>
   </si>
@@ -216,6 +216,17 @@
   <si>
     <t>PointersInC.txt
 ComditionalStatementsInC.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. I have completed 10 programs on Arrays from the given list of C questions and pushed the programs into git https://github.com/gandepallipavani/C_Programs
+2. Gone through the ppt shared by Srinivasa regarding SDLC and STLC taining 
+3. Attended the session by Srinivas about validating the testcases written
+4. Completed 3 hacker rank programs and pushed to git </t>
+  </si>
+  <si>
+    <t>PriningTokens.txt
+Sum&amp;Diff.txt
+PlaywithCharacters.txt</t>
   </si>
 </sst>
 </file>
@@ -639,10 +650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,6 +882,17 @@
         <v>46</v>
       </c>
     </row>
+    <row r="25" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <v>44257</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Pavani Gandepalli status on 4th Feb 2021
</commit_message>
<xml_diff>
--- a/PavaniGandepalli/Pavani_Gandepalli_B&I_StatusSheet.xlsx
+++ b/PavaniGandepalli/Pavani_Gandepalli_B&I_StatusSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Date</t>
   </si>
@@ -227,6 +227,21 @@
     <t>PriningTokens.txt
 Sum&amp;Diff.txt
 PlaywithCharacters.txt</t>
+  </si>
+  <si>
+    <t>StudentMarksSum.txt</t>
+  </si>
+  <si>
+    <t>1. I have completed bitwise operators 7 programs, pointers 2 programs from given list of programs and pushed to github
+https://github.com/gandepallipavani/C_Programs
+2. Gone through interview questions 
+ a. Compilation steps
+ b. Memory layout 
+ c. storage classes
+ d. Local static and global static
+ e. Bitwise
+3. Gone through test case parameters and bug life cycle slides in testing ppt shared by Srinivasa
+4. I have completed 1 hacker rank program</t>
   </si>
 </sst>
 </file>
@@ -313,9 +328,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -341,10 +355,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -650,26 +664,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="41.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="41.85546875" style="6" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
@@ -680,217 +694,223 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:5" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="3"/>
+      <c r="A6" s="5"/>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-    </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
+      <c r="A9" s="9">
         <v>44409</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
+      <c r="A10" s="9">
         <v>44501</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
+      <c r="A11" s="9">
         <v>44531</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="180" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="2" t="s">
+      <c r="C15" s="2"/>
+      <c r="D15" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="225" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="2" t="s">
+      <c r="C16" s="2"/>
+      <c r="D16" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="180" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3" t="s">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3" t="s">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="4"/>
+      <c r="F21" s="3"/>
     </row>
     <row r="22" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="180" x14ac:dyDescent="0.25">
-      <c r="A23" s="10">
+      <c r="A23" s="9">
         <v>44198</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="180" x14ac:dyDescent="0.25">
-      <c r="A24" s="10">
+      <c r="A24" s="9">
         <v>44229</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="165" x14ac:dyDescent="0.25">
-      <c r="A25" s="10">
+      <c r="A25" s="9">
         <v>44257</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="1" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="225" x14ac:dyDescent="0.25">
+      <c r="A26" s="9">
+        <v>44288</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pavani Gandepalli status on 5/2/2021
</commit_message>
<xml_diff>
--- a/PavaniGandepalli/Pavani_Gandepalli_B&I_StatusSheet.xlsx
+++ b/PavaniGandepalli/Pavani_Gandepalli_B&I_StatusSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Date</t>
   </si>
@@ -242,6 +242,20 @@
  e. Bitwise
 3. Gone through test case parameters and bug life cycle slides in testing ppt shared by Srinivasa
 4. I have completed 1 hacker rank program</t>
+  </si>
+  <si>
+    <t>1. I have completed pointers 5 programs and 2 files programs from given list of programs and pushed to GitHub
+https://github.com/gandepallipavani/C_Programs
+2. Gone through interview questions 
+ a. Size of structure without using sizeof operator
+ b. If (0), if (-1)
+ c. Call by value and call by reference
+3. Gone through testing ppt shared by Srinivasa
+4. I have completed 2 hacker rank programs today</t>
+  </si>
+  <si>
+    <t>forinC.txt
+Sumof5Digit.txt</t>
   </si>
 </sst>
 </file>
@@ -664,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,6 +927,17 @@
         <v>49</v>
       </c>
     </row>
+    <row r="27" spans="1:6" ht="225" x14ac:dyDescent="0.25">
+      <c r="A27" s="9">
+        <v>44318</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>